<commit_message>
Create expected case number 6 after cleaning time index.
</commit_message>
<xml_diff>
--- a/tests/strategies/clean/expected/test_case6.xlsx
+++ b/tests/strategies/clean/expected/test_case6.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="VAB K" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="114210"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -386,9 +386,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -402,9 +399,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -417,6 +411,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -426,8 +423,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -734,13 +734,13 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:BI36"/>
+  <dimension ref="A1:BJ36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.65" x14ac:dyDescent="0.3"/>
@@ -768,215 +768,341 @@
     <col min="57" max="61" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:62" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="33"/>
     </row>
-    <row r="2" spans="1:61" s="3" customFormat="1" ht="11.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:62" s="3" customFormat="1" ht="11.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
     </row>
-    <row r="3" spans="1:61" s="4" customFormat="1" ht="11.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:62" s="4" customFormat="1" ht="11.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
     </row>
-    <row r="4" spans="1:61" s="4" customFormat="1" ht="11.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:62" s="4" customFormat="1" ht="11.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="27">
-        <v>2004</v>
-      </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="27">
-        <v>2005</v>
-      </c>
-      <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="27">
-        <v>2006</v>
-      </c>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="27"/>
-      <c r="T4" s="20"/>
-      <c r="U4" s="27">
-        <v>2007</v>
-      </c>
-      <c r="V4" s="27"/>
-      <c r="W4" s="27"/>
-      <c r="X4" s="27"/>
-      <c r="Y4" s="27"/>
-      <c r="Z4" s="20"/>
-      <c r="AA4" s="27">
-        <v>2008</v>
-      </c>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="27"/>
-      <c r="AE4" s="27"/>
-      <c r="AF4" s="20"/>
-      <c r="AG4" s="27">
-        <v>2009</v>
-      </c>
-      <c r="AH4" s="27"/>
-      <c r="AI4" s="27"/>
-      <c r="AJ4" s="27"/>
-      <c r="AK4" s="27"/>
-      <c r="AL4" s="20"/>
-      <c r="AM4" s="27">
-        <v>2010</v>
-      </c>
-      <c r="AN4" s="27"/>
-      <c r="AO4" s="27"/>
-      <c r="AP4" s="27"/>
-      <c r="AQ4" s="27"/>
-      <c r="AR4" s="20"/>
-      <c r="AS4" s="27">
-        <v>2011</v>
-      </c>
-      <c r="AT4" s="27"/>
-      <c r="AU4" s="27"/>
-      <c r="AV4" s="27"/>
-      <c r="AW4" s="27"/>
-      <c r="AX4" s="20"/>
-      <c r="AY4" s="27">
-        <v>2012</v>
-      </c>
-      <c r="AZ4" s="27"/>
-      <c r="BA4" s="27"/>
-      <c r="BB4" s="27"/>
-      <c r="BC4" s="27"/>
-      <c r="BD4" s="20"/>
-      <c r="BE4" s="27">
-        <v>2013</v>
-      </c>
-      <c r="BF4" s="27"/>
-      <c r="BG4" s="27"/>
-      <c r="BH4" s="27"/>
-      <c r="BI4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="34">
+        <v>37987</v>
+      </c>
+      <c r="D4" s="34">
+        <v>37987</v>
+      </c>
+      <c r="E4" s="34">
+        <v>38078</v>
+      </c>
+      <c r="F4" s="34">
+        <v>38169</v>
+      </c>
+      <c r="G4" s="34">
+        <v>38261</v>
+      </c>
+      <c r="H4" s="23"/>
+      <c r="I4" s="34">
+        <f>DATE(YEAR(C4)+1,MONTH(C4),1)</f>
+        <v>38353</v>
+      </c>
+      <c r="J4" s="34">
+        <f t="shared" ref="J4:M4" si="0">DATE(YEAR(D4)+1,MONTH(D4),1)</f>
+        <v>38353</v>
+      </c>
+      <c r="K4" s="34">
+        <f t="shared" si="0"/>
+        <v>38443</v>
+      </c>
+      <c r="L4" s="34">
+        <f t="shared" si="0"/>
+        <v>38534</v>
+      </c>
+      <c r="M4" s="34">
+        <f t="shared" si="0"/>
+        <v>38626</v>
+      </c>
+      <c r="N4" s="23"/>
+      <c r="O4" s="34">
+        <f>DATE(YEAR(I4)+1,MONTH(I4),1)</f>
+        <v>38718</v>
+      </c>
+      <c r="P4" s="34">
+        <f t="shared" ref="P4" si="1">DATE(YEAR(J4)+1,MONTH(J4),1)</f>
+        <v>38718</v>
+      </c>
+      <c r="Q4" s="34">
+        <f t="shared" ref="Q4" si="2">DATE(YEAR(K4)+1,MONTH(K4),1)</f>
+        <v>38808</v>
+      </c>
+      <c r="R4" s="34">
+        <f t="shared" ref="R4" si="3">DATE(YEAR(L4)+1,MONTH(L4),1)</f>
+        <v>38899</v>
+      </c>
+      <c r="S4" s="34">
+        <f t="shared" ref="S4" si="4">DATE(YEAR(M4)+1,MONTH(M4),1)</f>
+        <v>38991</v>
+      </c>
+      <c r="T4" s="23"/>
+      <c r="U4" s="34">
+        <f>DATE(YEAR(O4)+1,MONTH(O4),1)</f>
+        <v>39083</v>
+      </c>
+      <c r="V4" s="34">
+        <f t="shared" ref="V4" si="5">DATE(YEAR(P4)+1,MONTH(P4),1)</f>
+        <v>39083</v>
+      </c>
+      <c r="W4" s="34">
+        <f t="shared" ref="W4" si="6">DATE(YEAR(Q4)+1,MONTH(Q4),1)</f>
+        <v>39173</v>
+      </c>
+      <c r="X4" s="34">
+        <f t="shared" ref="X4" si="7">DATE(YEAR(R4)+1,MONTH(R4),1)</f>
+        <v>39264</v>
+      </c>
+      <c r="Y4" s="34">
+        <f t="shared" ref="Y4" si="8">DATE(YEAR(S4)+1,MONTH(S4),1)</f>
+        <v>39356</v>
+      </c>
+      <c r="Z4" s="23"/>
+      <c r="AA4" s="34">
+        <f t="shared" ref="AA4" si="9">DATE(YEAR(U4)+1,MONTH(U4),1)</f>
+        <v>39448</v>
+      </c>
+      <c r="AB4" s="34">
+        <f t="shared" ref="AB4" si="10">DATE(YEAR(V4)+1,MONTH(V4),1)</f>
+        <v>39448</v>
+      </c>
+      <c r="AC4" s="34">
+        <f t="shared" ref="AC4" si="11">DATE(YEAR(W4)+1,MONTH(W4),1)</f>
+        <v>39539</v>
+      </c>
+      <c r="AD4" s="34">
+        <f t="shared" ref="AD4" si="12">DATE(YEAR(X4)+1,MONTH(X4),1)</f>
+        <v>39630</v>
+      </c>
+      <c r="AE4" s="34">
+        <f t="shared" ref="AE4" si="13">DATE(YEAR(Y4)+1,MONTH(Y4),1)</f>
+        <v>39722</v>
+      </c>
+      <c r="AF4" s="23"/>
+      <c r="AG4" s="34">
+        <f t="shared" ref="AG4" si="14">DATE(YEAR(AA4)+1,MONTH(AA4),1)</f>
+        <v>39814</v>
+      </c>
+      <c r="AH4" s="34">
+        <f t="shared" ref="AH4" si="15">DATE(YEAR(AB4)+1,MONTH(AB4),1)</f>
+        <v>39814</v>
+      </c>
+      <c r="AI4" s="34">
+        <f t="shared" ref="AI4" si="16">DATE(YEAR(AC4)+1,MONTH(AC4),1)</f>
+        <v>39904</v>
+      </c>
+      <c r="AJ4" s="34">
+        <f t="shared" ref="AJ4" si="17">DATE(YEAR(AD4)+1,MONTH(AD4),1)</f>
+        <v>39995</v>
+      </c>
+      <c r="AK4" s="34">
+        <f t="shared" ref="AK4" si="18">DATE(YEAR(AE4)+1,MONTH(AE4),1)</f>
+        <v>40087</v>
+      </c>
+      <c r="AL4" s="23"/>
+      <c r="AM4" s="34">
+        <f t="shared" ref="AM4" si="19">DATE(YEAR(AG4)+1,MONTH(AG4),1)</f>
+        <v>40179</v>
+      </c>
+      <c r="AN4" s="34">
+        <f t="shared" ref="AN4" si="20">DATE(YEAR(AH4)+1,MONTH(AH4),1)</f>
+        <v>40179</v>
+      </c>
+      <c r="AO4" s="34">
+        <f t="shared" ref="AO4" si="21">DATE(YEAR(AI4)+1,MONTH(AI4),1)</f>
+        <v>40269</v>
+      </c>
+      <c r="AP4" s="34">
+        <f t="shared" ref="AP4" si="22">DATE(YEAR(AJ4)+1,MONTH(AJ4),1)</f>
+        <v>40360</v>
+      </c>
+      <c r="AQ4" s="34">
+        <f t="shared" ref="AQ4" si="23">DATE(YEAR(AK4)+1,MONTH(AK4),1)</f>
+        <v>40452</v>
+      </c>
+      <c r="AR4" s="23"/>
+      <c r="AS4" s="34">
+        <f t="shared" ref="AS4" si="24">DATE(YEAR(AM4)+1,MONTH(AM4),1)</f>
+        <v>40544</v>
+      </c>
+      <c r="AT4" s="34">
+        <f t="shared" ref="AT4" si="25">DATE(YEAR(AN4)+1,MONTH(AN4),1)</f>
+        <v>40544</v>
+      </c>
+      <c r="AU4" s="34">
+        <f t="shared" ref="AU4" si="26">DATE(YEAR(AO4)+1,MONTH(AO4),1)</f>
+        <v>40634</v>
+      </c>
+      <c r="AV4" s="34">
+        <f t="shared" ref="AV4" si="27">DATE(YEAR(AP4)+1,MONTH(AP4),1)</f>
+        <v>40725</v>
+      </c>
+      <c r="AW4" s="34">
+        <f t="shared" ref="AW4" si="28">DATE(YEAR(AQ4)+1,MONTH(AQ4),1)</f>
+        <v>40817</v>
+      </c>
+      <c r="AX4" s="23"/>
+      <c r="AY4" s="34">
+        <f t="shared" ref="AY4" si="29">DATE(YEAR(AS4)+1,MONTH(AS4),1)</f>
+        <v>40909</v>
+      </c>
+      <c r="AZ4" s="34">
+        <f t="shared" ref="AZ4" si="30">DATE(YEAR(AT4)+1,MONTH(AT4),1)</f>
+        <v>40909</v>
+      </c>
+      <c r="BA4" s="34">
+        <f t="shared" ref="BA4" si="31">DATE(YEAR(AU4)+1,MONTH(AU4),1)</f>
+        <v>41000</v>
+      </c>
+      <c r="BB4" s="34">
+        <f t="shared" ref="BB4" si="32">DATE(YEAR(AV4)+1,MONTH(AV4),1)</f>
+        <v>41091</v>
+      </c>
+      <c r="BC4" s="34">
+        <f t="shared" ref="BC4" si="33">DATE(YEAR(AW4)+1,MONTH(AW4),1)</f>
+        <v>41183</v>
+      </c>
+      <c r="BD4" s="23"/>
+      <c r="BE4" s="34">
+        <f t="shared" ref="BE4" si="34">DATE(YEAR(AY4)+1,MONTH(AY4),1)</f>
+        <v>41275</v>
+      </c>
+      <c r="BF4" s="34">
+        <f t="shared" ref="BF4" si="35">DATE(YEAR(AZ4)+1,MONTH(AZ4),1)</f>
+        <v>41275</v>
+      </c>
+      <c r="BG4" s="34">
+        <f t="shared" ref="BG4" si="36">DATE(YEAR(BA4)+1,MONTH(BA4),1)</f>
+        <v>41365</v>
+      </c>
+      <c r="BH4" s="34">
+        <f t="shared" ref="BH4" si="37">DATE(YEAR(BB4)+1,MONTH(BB4),1)</f>
+        <v>41456</v>
+      </c>
+      <c r="BI4" s="34">
+        <f t="shared" ref="BI4" si="38">DATE(YEAR(BC4)+1,MONTH(BC4),1)</f>
+        <v>41548</v>
+      </c>
+      <c r="BJ4" s="23"/>
     </row>
-    <row r="5" spans="1:61" s="4" customFormat="1" ht="10.85" x14ac:dyDescent="0.2">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="24" t="s">
+    <row r="5" spans="1:62" s="4" customFormat="1" ht="10.85" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
       <c r="H5" s="17"/>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
       <c r="N5" s="17"/>
-      <c r="O5" s="24" t="s">
+      <c r="O5" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="P5" s="28" t="s">
+      <c r="P5" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28"/>
-      <c r="S5" s="28"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
       <c r="T5" s="17"/>
-      <c r="U5" s="24" t="s">
+      <c r="U5" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="V5" s="28" t="s">
+      <c r="V5" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="W5" s="28"/>
-      <c r="X5" s="28"/>
-      <c r="Y5" s="28"/>
+      <c r="W5" s="26"/>
+      <c r="X5" s="26"/>
+      <c r="Y5" s="26"/>
       <c r="Z5" s="17"/>
-      <c r="AA5" s="24" t="s">
+      <c r="AA5" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="AB5" s="28" t="s">
+      <c r="AB5" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AC5" s="28"/>
-      <c r="AD5" s="28"/>
-      <c r="AE5" s="28"/>
+      <c r="AC5" s="26"/>
+      <c r="AD5" s="26"/>
+      <c r="AE5" s="26"/>
       <c r="AF5" s="17"/>
-      <c r="AG5" s="24" t="s">
+      <c r="AG5" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="AH5" s="28" t="s">
+      <c r="AH5" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AI5" s="28"/>
-      <c r="AJ5" s="28"/>
-      <c r="AK5" s="28"/>
+      <c r="AI5" s="26"/>
+      <c r="AJ5" s="26"/>
+      <c r="AK5" s="26"/>
       <c r="AL5" s="17"/>
-      <c r="AM5" s="24" t="s">
+      <c r="AM5" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="AN5" s="28" t="s">
+      <c r="AN5" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AO5" s="28"/>
-      <c r="AP5" s="28"/>
-      <c r="AQ5" s="28"/>
+      <c r="AO5" s="26"/>
+      <c r="AP5" s="26"/>
+      <c r="AQ5" s="26"/>
       <c r="AR5" s="17"/>
-      <c r="AS5" s="24" t="s">
+      <c r="AS5" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="AT5" s="28" t="s">
+      <c r="AT5" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AU5" s="28"/>
-      <c r="AV5" s="28"/>
-      <c r="AW5" s="28"/>
+      <c r="AU5" s="26"/>
+      <c r="AV5" s="26"/>
+      <c r="AW5" s="26"/>
       <c r="AX5" s="17"/>
-      <c r="AY5" s="24" t="s">
+      <c r="AY5" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="AZ5" s="28" t="s">
+      <c r="AZ5" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="BA5" s="28"/>
-      <c r="BB5" s="28"/>
-      <c r="BC5" s="28"/>
+      <c r="BA5" s="26"/>
+      <c r="BB5" s="26"/>
+      <c r="BC5" s="26"/>
       <c r="BD5" s="17"/>
-      <c r="BE5" s="24" t="s">
+      <c r="BE5" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="BF5" s="27" t="s">
+      <c r="BF5" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="BG5" s="27"/>
-      <c r="BH5" s="27"/>
-      <c r="BI5" s="27"/>
+      <c r="BG5" s="25"/>
+      <c r="BH5" s="25"/>
+      <c r="BI5" s="25"/>
     </row>
-    <row r="6" spans="1:61" s="9" customFormat="1" ht="11.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
+    <row r="6" spans="1:62" s="9" customFormat="1" ht="11.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="16" t="s">
         <v>44</v>
       </c>
@@ -990,7 +1116,7 @@
         <v>47</v>
       </c>
       <c r="H6" s="16"/>
-      <c r="I6" s="25"/>
+      <c r="I6" s="24"/>
       <c r="J6" s="16" t="s">
         <v>52</v>
       </c>
@@ -1004,7 +1130,7 @@
         <v>55</v>
       </c>
       <c r="N6" s="16"/>
-      <c r="O6" s="25"/>
+      <c r="O6" s="24"/>
       <c r="P6" s="16" t="s">
         <v>50</v>
       </c>
@@ -1018,7 +1144,7 @@
         <v>51</v>
       </c>
       <c r="T6" s="16"/>
-      <c r="U6" s="25"/>
+      <c r="U6" s="24"/>
       <c r="V6" s="16" t="s">
         <v>50</v>
       </c>
@@ -1032,7 +1158,7 @@
         <v>51</v>
       </c>
       <c r="Z6" s="16"/>
-      <c r="AA6" s="25"/>
+      <c r="AA6" s="24"/>
       <c r="AB6" s="16" t="s">
         <v>50</v>
       </c>
@@ -1046,7 +1172,7 @@
         <v>51</v>
       </c>
       <c r="AF6" s="16"/>
-      <c r="AG6" s="25"/>
+      <c r="AG6" s="24"/>
       <c r="AH6" s="16" t="s">
         <v>50</v>
       </c>
@@ -1060,7 +1186,7 @@
         <v>51</v>
       </c>
       <c r="AL6" s="16"/>
-      <c r="AM6" s="25"/>
+      <c r="AM6" s="24"/>
       <c r="AN6" s="16" t="s">
         <v>50</v>
       </c>
@@ -1074,7 +1200,7 @@
         <v>51</v>
       </c>
       <c r="AR6" s="16"/>
-      <c r="AS6" s="25"/>
+      <c r="AS6" s="24"/>
       <c r="AT6" s="16" t="s">
         <v>50</v>
       </c>
@@ -1088,7 +1214,7 @@
         <v>51</v>
       </c>
       <c r="AX6" s="16"/>
-      <c r="AY6" s="25"/>
+      <c r="AY6" s="24"/>
       <c r="AZ6" s="16" t="s">
         <v>50</v>
       </c>
@@ -1102,7 +1228,7 @@
         <v>51</v>
       </c>
       <c r="BD6" s="16"/>
-      <c r="BE6" s="34"/>
+      <c r="BE6" s="29"/>
       <c r="BF6" s="16" t="s">
         <v>56</v>
       </c>
@@ -1116,7 +1242,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:61" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:62" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="14"/>
@@ -1179,7 +1305,7 @@
       <c r="BH7" s="15"/>
       <c r="BI7" s="15"/>
     </row>
-    <row r="8" spans="1:61" s="4" customFormat="1" ht="21.7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:62" s="4" customFormat="1" ht="21.7" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
@@ -1346,7 +1472,7 @@
         <v>68436900.413885087</v>
       </c>
     </row>
-    <row r="9" spans="1:61" s="4" customFormat="1" ht="10.85" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:62" s="4" customFormat="1" ht="10.85" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
@@ -1513,7 +1639,7 @@
         <v>1954239.8919898374</v>
       </c>
     </row>
-    <row r="10" spans="1:61" s="4" customFormat="1" ht="10.85" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:62" s="4" customFormat="1" ht="10.85" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
@@ -1680,7 +1806,7 @@
         <v>24783319.435808077</v>
       </c>
     </row>
-    <row r="11" spans="1:61" s="4" customFormat="1" ht="10.85" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:62" s="4" customFormat="1" ht="10.85" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
@@ -1847,7 +1973,7 @@
         <v>175568594.8187896</v>
       </c>
     </row>
-    <row r="12" spans="1:61" s="4" customFormat="1" ht="10.85" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:62" s="4" customFormat="1" ht="10.85" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
@@ -2014,7 +2140,7 @@
         <v>12044770.034440761</v>
       </c>
     </row>
-    <row r="13" spans="1:61" s="4" customFormat="1" ht="10.85" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:62" s="4" customFormat="1" ht="10.85" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -2181,7 +2307,7 @@
         <v>38529801.535895616</v>
       </c>
     </row>
-    <row r="14" spans="1:61" s="4" customFormat="1" ht="21.7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:62" s="4" customFormat="1" ht="21.7" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
@@ -2348,7 +2474,7 @@
         <v>131262967.08849336</v>
       </c>
     </row>
-    <row r="15" spans="1:61" s="4" customFormat="1" ht="10.85" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:62" s="4" customFormat="1" ht="10.85" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
@@ -2515,7 +2641,7 @@
         <v>22298470.832997486</v>
       </c>
     </row>
-    <row r="16" spans="1:61" s="4" customFormat="1" ht="10.85" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:62" s="4" customFormat="1" ht="10.85" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
@@ -4526,163 +4652,163 @@
       <c r="B28" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="21">
+      <c r="C28" s="20">
         <v>535828336.44026625</v>
       </c>
-      <c r="D28" s="21">
+      <c r="D28" s="20">
         <v>500791684.03710359</v>
       </c>
-      <c r="E28" s="21">
+      <c r="E28" s="20">
         <v>540780075.80782855</v>
       </c>
-      <c r="F28" s="21">
+      <c r="F28" s="20">
         <v>532335833.36363554</v>
       </c>
-      <c r="G28" s="21">
+      <c r="G28" s="20">
         <v>569405752.55249631</v>
       </c>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21">
+      <c r="H28" s="20"/>
+      <c r="I28" s="20">
         <v>585116446.86535442</v>
       </c>
-      <c r="J28" s="21">
+      <c r="J28" s="20">
         <v>538633210.03692508</v>
       </c>
-      <c r="K28" s="21">
+      <c r="K28" s="20">
         <v>602457546.84444702</v>
       </c>
-      <c r="L28" s="21">
+      <c r="L28" s="20">
         <v>579373903.70794225</v>
       </c>
-      <c r="M28" s="21">
+      <c r="M28" s="20">
         <v>620001126.8721031</v>
       </c>
-      <c r="N28" s="21"/>
-      <c r="O28" s="21">
+      <c r="N28" s="20"/>
+      <c r="O28" s="20">
         <v>634055144.16104412</v>
       </c>
-      <c r="P28" s="21">
+      <c r="P28" s="20">
         <v>585883448.77654517</v>
       </c>
-      <c r="Q28" s="21">
+      <c r="Q28" s="20">
         <v>648923104.03840971</v>
       </c>
-      <c r="R28" s="21">
+      <c r="R28" s="20">
         <v>630430265.00448048</v>
       </c>
-      <c r="S28" s="21">
+      <c r="S28" s="20">
         <v>670983758.82474089</v>
       </c>
-      <c r="T28" s="21"/>
-      <c r="U28" s="21">
+      <c r="T28" s="20"/>
+      <c r="U28" s="20">
         <v>684797886.1733104</v>
       </c>
-      <c r="V28" s="21">
+      <c r="V28" s="20">
         <v>628278543.10002375</v>
       </c>
-      <c r="W28" s="21">
+      <c r="W28" s="20">
         <v>700471806.5225035</v>
       </c>
-      <c r="X28" s="21">
+      <c r="X28" s="20">
         <v>677507119.63955355</v>
       </c>
-      <c r="Y28" s="21">
+      <c r="Y28" s="20">
         <v>732934075.43116105</v>
       </c>
-      <c r="Z28" s="21"/>
-      <c r="AA28" s="21">
+      <c r="Z28" s="20"/>
+      <c r="AA28" s="20">
         <v>706041092.10255694</v>
       </c>
-      <c r="AB28" s="21">
+      <c r="AB28" s="20">
         <v>665533554.8137877</v>
       </c>
-      <c r="AC28" s="21">
+      <c r="AC28" s="20">
         <v>731078301.00297344</v>
       </c>
-      <c r="AD28" s="21">
+      <c r="AD28" s="20">
         <v>714978419.8057369</v>
       </c>
-      <c r="AE28" s="21">
+      <c r="AE28" s="20">
         <v>712574092.78772998</v>
       </c>
-      <c r="AF28" s="21"/>
-      <c r="AG28" s="21">
+      <c r="AF28" s="20"/>
+      <c r="AG28" s="20">
         <v>706397733.38573241</v>
       </c>
-      <c r="AH28" s="21">
+      <c r="AH28" s="20">
         <v>663167773.79222775</v>
       </c>
-      <c r="AI28" s="21">
+      <c r="AI28" s="20">
         <v>705410535.39351642</v>
       </c>
-      <c r="AJ28" s="21">
+      <c r="AJ28" s="20">
         <v>702663243.26136577</v>
       </c>
-      <c r="AK28" s="21">
+      <c r="AK28" s="20">
         <v>754349381.09581947</v>
       </c>
-      <c r="AL28" s="21"/>
-      <c r="AM28" s="21">
+      <c r="AL28" s="20"/>
+      <c r="AM28" s="20">
         <v>770935939.9576292</v>
       </c>
-      <c r="AN28" s="21">
+      <c r="AN28" s="20">
         <v>696858816.45135248</v>
       </c>
-      <c r="AO28" s="21">
+      <c r="AO28" s="20">
         <v>790558446.49510336</v>
       </c>
-      <c r="AP28" s="21">
+      <c r="AP28" s="20">
         <v>776240103.96728218</v>
       </c>
-      <c r="AQ28" s="21">
+      <c r="AQ28" s="20">
         <v>820086392.91677892</v>
       </c>
-      <c r="AR28" s="21"/>
-      <c r="AS28" s="21">
+      <c r="AR28" s="20"/>
+      <c r="AS28" s="20">
         <v>836888837.04314756</v>
       </c>
-      <c r="AT28" s="21">
+      <c r="AT28" s="20">
         <v>771371200.02394903</v>
       </c>
-      <c r="AU28" s="21">
+      <c r="AU28" s="20">
         <v>854542030.21858263</v>
       </c>
-      <c r="AV28" s="21">
+      <c r="AV28" s="20">
         <v>842001110.49020493</v>
       </c>
-      <c r="AW28" s="21">
+      <c r="AW28" s="20">
         <v>879641007.43985331</v>
       </c>
-      <c r="AX28" s="21"/>
-      <c r="AY28" s="21">
+      <c r="AX28" s="20"/>
+      <c r="AY28" s="20">
         <v>844807455.40952492</v>
       </c>
-      <c r="AZ28" s="21">
+      <c r="AZ28" s="20">
         <v>806494630.69455087</v>
       </c>
-      <c r="BA28" s="21">
+      <c r="BA28" s="20">
         <v>841495946.26784444</v>
       </c>
-      <c r="BB28" s="21">
+      <c r="BB28" s="20">
         <v>843413968.90232086</v>
       </c>
-      <c r="BC28" s="21">
+      <c r="BC28" s="20">
         <v>887825275.77338386</v>
       </c>
-      <c r="BD28" s="21"/>
-      <c r="BE28" s="21">
+      <c r="BD28" s="20"/>
+      <c r="BE28" s="20">
         <v>869739469.91282988</v>
       </c>
-      <c r="BF28" s="21">
+      <c r="BF28" s="20">
         <v>818437956.0566839</v>
       </c>
-      <c r="BG28" s="21">
+      <c r="BG28" s="20">
         <v>887532750.08222568</v>
       </c>
-      <c r="BH28" s="21">
+      <c r="BH28" s="20">
         <v>873154515.6651839</v>
       </c>
-      <c r="BI28" s="21">
+      <c r="BI28" s="20">
         <v>899832657.84722626</v>
       </c>
     </row>
@@ -4750,10 +4876,10 @@
       <c r="BI29" s="12"/>
     </row>
     <row r="30" spans="1:61" s="4" customFormat="1" ht="13.55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="32"/>
+      <c r="B30" s="31"/>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
@@ -4815,26 +4941,26 @@
       <c r="BI30" s="12"/>
     </row>
     <row r="31" spans="1:61" s="4" customFormat="1" ht="11.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="32"/>
+      <c r="B31" s="31"/>
     </row>
     <row r="32" spans="1:61" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="32"/>
+      <c r="B32" s="31"/>
     </row>
     <row r="33" spans="1:2" s="4" customFormat="1" ht="10.85" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
       <c r="B33" s="6"/>
     </row>
     <row r="34" spans="1:2" s="4" customFormat="1" ht="13.55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="33" t="s">
+      <c r="A34" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="32"/>
+      <c r="B34" s="31"/>
     </row>
     <row r="35" spans="1:2" s="4" customFormat="1" ht="10.85" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
@@ -4845,43 +4971,12 @@
       <c r="B36" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="36">
-    <mergeCell ref="BE5:BE6"/>
-    <mergeCell ref="BE4:BI4"/>
-    <mergeCell ref="BF5:BI5"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="AY4:BC4"/>
-    <mergeCell ref="I4:M4"/>
-    <mergeCell ref="AM4:AQ4"/>
-    <mergeCell ref="O4:S4"/>
-    <mergeCell ref="AN5:AQ5"/>
-    <mergeCell ref="AG4:AK4"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="AS4:AW4"/>
-    <mergeCell ref="AS5:AS6"/>
-    <mergeCell ref="AT5:AW5"/>
-    <mergeCell ref="AA4:AE4"/>
-    <mergeCell ref="AA5:AA6"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="U4:Y4"/>
-    <mergeCell ref="V5:Y5"/>
-    <mergeCell ref="AB5:AE5"/>
+  <mergeCells count="5">
+    <mergeCell ref="A1:B1"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A34:B34"/>
-    <mergeCell ref="AY5:AY6"/>
-    <mergeCell ref="AZ5:BC5"/>
-    <mergeCell ref="AG5:AG6"/>
-    <mergeCell ref="AH5:AK5"/>
-    <mergeCell ref="AM5:AM6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:S5"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="U5:U6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="A4:B6"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A30:B30"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>